<commit_message>
Add respective columns to output excel file
</commit_message>
<xml_diff>
--- a/files/Domain Tracking.xlsx
+++ b/files/Domain Tracking.xlsx
@@ -4,20 +4,23 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Domain" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Subscriptions" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="active-sites" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Subscriptions" sheetId="3" r:id="rId6"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Domain!$B$2:$N$74</definedName>
+  </definedNames>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="Yt3iAvGHFBytCgj9zcK5ULtFeeoWsbSc1zMCaIXl8ds="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="yvguSBR1dZAc3r746/gPgy8GG5oAyi0trwXqsWfx4AY="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="127">
   <si>
     <t>ACTIVE DOMAIN TRACKING</t>
   </si>
@@ -318,6 +321,12 @@
     <t>pelicancredit.co.ke</t>
   </si>
   <si>
+    <t>netduka.co.ke</t>
+  </si>
+  <si>
+    <t>netduka.com</t>
+  </si>
+  <si>
     <t>SUBSCRIPTION TRACKING</t>
   </si>
   <si>
@@ -414,7 +423,7 @@
     <numFmt numFmtId="166" formatCode="d&quot;-&quot;mmm&quot;-&quot;yyyy"/>
     <numFmt numFmtId="167" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="33">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -558,22 +567,16 @@
     <font>
       <u/>
       <sz val="11.0"/>
-      <color rgb="FF0563C1"/>
+      <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
     <font>
-      <u/>
-      <sz val="11.0"/>
-      <color rgb="FF0000FF"/>
-      <name val="Bookman Old Style"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
     </font>
     <font>
+      <b/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Bookman Old Style"/>
@@ -823,12 +826,10 @@
     <xf borderId="0" fillId="4" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="4" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -854,50 +855,50 @@
     <xf borderId="4" fillId="3" fontId="28" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="27" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="27" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="29" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="29" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="29" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="27" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="27" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="29" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="27" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="27" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="29" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="29" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -927,6 +928,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1313,14 +1318,14 @@
       <c r="I4" s="13"/>
       <c r="J4" s="16">
         <f t="shared" ref="J4:J74" si="1">TODAY()</f>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K4" s="18">
         <v>45413.0</v>
       </c>
       <c r="L4" s="17">
         <f t="shared" ref="L4:L74" si="2">K4-J4</f>
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="M4" s="17">
         <v>1549.76</v>
@@ -1373,14 +1378,14 @@
       <c r="I5" s="13"/>
       <c r="J5" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K5" s="18">
         <v>45413.0</v>
       </c>
       <c r="L5" s="17">
         <f t="shared" si="2"/>
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="M5" s="17">
         <v>1740.0</v>
@@ -1433,14 +1438,14 @@
       <c r="I6" s="13"/>
       <c r="J6" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K6" s="16">
         <v>45706.0</v>
       </c>
       <c r="L6" s="17">
         <f t="shared" si="2"/>
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="M6" s="17">
         <v>3480.0</v>
@@ -1469,7 +1474,7 @@
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
     </row>
-    <row r="7">
+    <row r="7" hidden="1">
       <c r="A7" s="1"/>
       <c r="B7" s="17">
         <v>4.0</v>
@@ -1493,14 +1498,14 @@
       <c r="I7" s="13"/>
       <c r="J7" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K7" s="18">
         <v>45422.0</v>
       </c>
       <c r="L7" s="17">
         <f t="shared" si="2"/>
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="M7" s="17">
         <v>1740.0</v>
@@ -1529,7 +1534,7 @@
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" hidden="1">
       <c r="A8" s="1"/>
       <c r="B8" s="13">
         <v>5.0</v>
@@ -1555,14 +1560,14 @@
       </c>
       <c r="J8" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K8" s="16">
         <v>45237.0</v>
       </c>
       <c r="L8" s="17">
         <f t="shared" si="2"/>
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="M8" s="17">
         <v>1549.76</v>
@@ -1617,14 +1622,14 @@
       </c>
       <c r="J9" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K9" s="16">
         <v>45237.0</v>
       </c>
       <c r="L9" s="17">
         <f t="shared" si="2"/>
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="M9" s="17">
         <v>1740.0</v>
@@ -1677,14 +1682,14 @@
       <c r="I10" s="13"/>
       <c r="J10" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K10" s="16">
         <v>45150.0</v>
       </c>
       <c r="L10" s="17">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="M10" s="17">
         <v>1549.76</v>
@@ -1737,14 +1742,14 @@
       <c r="I11" s="13"/>
       <c r="J11" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K11" s="18">
         <v>45721.0</v>
       </c>
       <c r="L11" s="17">
         <f t="shared" si="2"/>
-        <v>597</v>
+        <v>590</v>
       </c>
       <c r="M11" s="17">
         <v>2900.0</v>
@@ -1773,7 +1778,7 @@
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
     </row>
-    <row r="12">
+    <row r="12" hidden="1">
       <c r="A12" s="1"/>
       <c r="B12" s="13">
         <v>9.0</v>
@@ -1799,14 +1804,14 @@
       </c>
       <c r="J12" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K12" s="18">
         <v>45189.0</v>
       </c>
       <c r="L12" s="17">
         <f t="shared" si="2"/>
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="M12" s="17">
         <v>1392.0</v>
@@ -1861,14 +1866,14 @@
       </c>
       <c r="J13" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K13" s="18">
         <v>45189.0</v>
       </c>
       <c r="L13" s="17">
         <f t="shared" si="2"/>
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="M13" s="17">
         <v>1740.0</v>
@@ -1921,14 +1926,14 @@
       <c r="I14" s="13"/>
       <c r="J14" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K14" s="18">
         <v>45198.0</v>
       </c>
       <c r="L14" s="17">
         <f t="shared" si="2"/>
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="M14" s="17">
         <v>1392.0</v>
@@ -1981,14 +1986,14 @@
       <c r="I15" s="13"/>
       <c r="J15" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K15" s="18">
         <v>45198.0</v>
       </c>
       <c r="L15" s="17">
         <f t="shared" si="2"/>
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="M15" s="17">
         <v>1740.0</v>
@@ -2017,7 +2022,7 @@
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
     </row>
-    <row r="16">
+    <row r="16" hidden="1">
       <c r="A16" s="1"/>
       <c r="B16" s="13">
         <v>13.0</v>
@@ -2041,14 +2046,14 @@
       <c r="I16" s="13"/>
       <c r="J16" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K16" s="18">
         <v>45198.0</v>
       </c>
       <c r="L16" s="17">
         <f t="shared" si="2"/>
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="M16" s="17">
         <v>1392.0</v>
@@ -2091,9 +2096,7 @@
       <c r="E17" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="18">
-        <v>44834.0</v>
-      </c>
+      <c r="F17" s="18"/>
       <c r="G17" s="17"/>
       <c r="H17" s="17" t="s">
         <v>32</v>
@@ -2101,14 +2104,14 @@
       <c r="I17" s="13"/>
       <c r="J17" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K17" s="18">
         <v>45198.0</v>
       </c>
       <c r="L17" s="17">
         <f t="shared" si="2"/>
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="M17" s="17">
         <v>1740.0</v>
@@ -2161,14 +2164,14 @@
       <c r="I18" s="13"/>
       <c r="J18" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K18" s="18">
         <v>45265.0</v>
       </c>
       <c r="L18" s="17">
         <f t="shared" si="2"/>
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="M18" s="17">
         <v>1392.0</v>
@@ -2221,14 +2224,14 @@
       <c r="I19" s="13"/>
       <c r="J19" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K19" s="18">
         <v>45355.0</v>
       </c>
       <c r="L19" s="17">
         <f t="shared" si="2"/>
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="M19" s="17">
         <v>1740.0</v>
@@ -2257,7 +2260,7 @@
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
     </row>
-    <row r="20">
+    <row r="20" hidden="1">
       <c r="A20" s="1"/>
       <c r="B20" s="13">
         <v>17.0</v>
@@ -2279,14 +2282,14 @@
       <c r="I20" s="13"/>
       <c r="J20" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K20" s="18">
         <v>45309.0</v>
       </c>
       <c r="L20" s="17">
         <f t="shared" si="2"/>
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="M20" s="17">
         <v>1392.0</v>
@@ -2335,14 +2338,14 @@
       <c r="I21" s="13"/>
       <c r="J21" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K21" s="18">
         <v>45309.0</v>
       </c>
       <c r="L21" s="17">
         <f t="shared" si="2"/>
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="M21" s="17">
         <v>1740.0</v>
@@ -2369,7 +2372,7 @@
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
     </row>
-    <row r="22">
+    <row r="22" hidden="1">
       <c r="A22" s="1"/>
       <c r="B22" s="13">
         <v>19.0</v>
@@ -2391,14 +2394,14 @@
       <c r="I22" s="13"/>
       <c r="J22" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K22" s="18">
         <v>45247.0</v>
       </c>
       <c r="L22" s="17">
         <f t="shared" si="2"/>
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="M22" s="17">
         <v>1740.0</v>
@@ -2425,7 +2428,7 @@
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" ht="15.75" hidden="1" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="17">
         <v>20.0</v>
@@ -2447,14 +2450,14 @@
       <c r="I23" s="13"/>
       <c r="J23" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K23" s="18">
         <v>45247.0</v>
       </c>
       <c r="L23" s="17">
         <f t="shared" si="2"/>
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="M23" s="17">
         <v>1740.0</v>
@@ -2505,14 +2508,14 @@
       <c r="I24" s="13"/>
       <c r="J24" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K24" s="18">
         <v>45265.0</v>
       </c>
       <c r="L24" s="17">
         <f t="shared" si="2"/>
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="M24" s="17">
         <v>1392.0</v>
@@ -2563,14 +2566,14 @@
       <c r="I25" s="13"/>
       <c r="J25" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K25" s="18">
         <v>45345.0</v>
       </c>
       <c r="L25" s="17">
         <f t="shared" si="2"/>
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="M25" s="17">
         <v>1740.0</v>
@@ -2599,7 +2602,7 @@
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" ht="15.75" hidden="1" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="13">
         <v>23.0</v>
@@ -2621,14 +2624,14 @@
       <c r="I26" s="13"/>
       <c r="J26" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K26" s="18">
         <v>45318.0</v>
       </c>
       <c r="L26" s="17">
         <f t="shared" si="2"/>
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="M26" s="17">
         <v>1740.0</v>
@@ -2679,14 +2682,14 @@
       <c r="I27" s="13"/>
       <c r="J27" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K27" s="18">
         <v>45494.0</v>
       </c>
       <c r="L27" s="17">
         <f t="shared" si="2"/>
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="M27" s="17">
         <v>1740.0</v>
@@ -2739,14 +2742,14 @@
       <c r="I28" s="13"/>
       <c r="J28" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K28" s="18">
         <v>45343.0</v>
       </c>
       <c r="L28" s="17">
         <f t="shared" si="2"/>
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="M28" s="17">
         <v>1740.0</v>
@@ -2775,7 +2778,7 @@
       <c r="AG28" s="1"/>
       <c r="AH28" s="1"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" ht="15.75" hidden="1" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="17">
         <v>26.0</v>
@@ -2797,14 +2800,14 @@
       <c r="I29" s="13"/>
       <c r="J29" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K29" s="18">
         <v>45338.0</v>
       </c>
       <c r="L29" s="17">
         <f t="shared" si="2"/>
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="M29" s="17">
         <v>1740.0</v>
@@ -2833,7 +2836,7 @@
       <c r="AG29" s="1"/>
       <c r="AH29" s="1"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" ht="15.75" hidden="1" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="13">
         <v>27.0</v>
@@ -2855,14 +2858,14 @@
       <c r="I30" s="13"/>
       <c r="J30" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K30" s="18">
         <v>45338.0</v>
       </c>
       <c r="L30" s="17">
         <f t="shared" si="2"/>
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="M30" s="17">
         <v>1740.0</v>
@@ -2891,7 +2894,7 @@
       <c r="AG30" s="1"/>
       <c r="AH30" s="1"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" ht="15.75" hidden="1" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="17">
         <v>28.0</v>
@@ -2913,14 +2916,14 @@
       <c r="I31" s="13"/>
       <c r="J31" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K31" s="18">
         <v>45349.0</v>
       </c>
       <c r="L31" s="17">
         <f t="shared" si="2"/>
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="M31" s="17">
         <v>1740.0</v>
@@ -2949,7 +2952,7 @@
       <c r="AG31" s="1"/>
       <c r="AH31" s="1"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" ht="15.75" hidden="1" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="13">
         <v>29.0</v>
@@ -2973,14 +2976,14 @@
       <c r="I32" s="13"/>
       <c r="J32" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K32" s="18">
         <v>45281.0</v>
       </c>
       <c r="L32" s="17">
         <f t="shared" si="2"/>
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="M32" s="17">
         <v>1740.0</v>
@@ -3009,7 +3012,7 @@
       <c r="AG32" s="1"/>
       <c r="AH32" s="1"/>
     </row>
-    <row r="33" ht="15.75" customHeight="1">
+    <row r="33" ht="15.75" hidden="1" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="17">
         <v>30.0</v>
@@ -3031,14 +3034,14 @@
       <c r="I33" s="13"/>
       <c r="J33" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K33" s="18">
         <v>45318.0</v>
       </c>
       <c r="L33" s="17">
         <f t="shared" si="2"/>
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="M33" s="17">
         <v>1740.0</v>
@@ -3067,7 +3070,7 @@
       <c r="AG33" s="1"/>
       <c r="AH33" s="1"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" ht="15.75" hidden="1" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="13">
         <v>31.0</v>
@@ -3089,14 +3092,14 @@
       <c r="I34" s="13"/>
       <c r="J34" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K34" s="18">
         <v>45343.0</v>
       </c>
       <c r="L34" s="17">
         <f t="shared" si="2"/>
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="M34" s="17">
         <v>1740.0</v>
@@ -3125,7 +3128,7 @@
       <c r="AG34" s="1"/>
       <c r="AH34" s="1"/>
     </row>
-    <row r="35" ht="15.75" customHeight="1">
+    <row r="35" ht="15.75" hidden="1" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="17">
         <v>32.0</v>
@@ -3147,14 +3150,14 @@
       <c r="I35" s="13"/>
       <c r="J35" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K35" s="18">
         <v>45343.0</v>
       </c>
       <c r="L35" s="17">
         <f t="shared" si="2"/>
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="M35" s="17">
         <v>1740.0</v>
@@ -3207,14 +3210,14 @@
       <c r="I36" s="13"/>
       <c r="J36" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K36" s="18">
         <v>45479.0</v>
       </c>
       <c r="L36" s="17">
         <f t="shared" si="2"/>
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="M36" s="17">
         <v>1740.0</v>
@@ -3265,14 +3268,14 @@
       <c r="I37" s="13"/>
       <c r="J37" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K37" s="18">
         <v>45328.0</v>
       </c>
       <c r="L37" s="17">
         <f t="shared" si="2"/>
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="M37" s="17">
         <v>1740.0</v>
@@ -3301,7 +3304,7 @@
       <c r="AG37" s="1"/>
       <c r="AH37" s="1"/>
     </row>
-    <row r="38" ht="15.75" customHeight="1">
+    <row r="38" ht="15.75" hidden="1" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="13">
         <v>35.0</v>
@@ -3323,14 +3326,14 @@
       <c r="I38" s="13"/>
       <c r="J38" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K38" s="18">
         <v>45312.0</v>
       </c>
       <c r="L38" s="17">
         <f t="shared" si="2"/>
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="M38" s="17">
         <v>1740.0</v>
@@ -3383,14 +3386,14 @@
       <c r="I39" s="13"/>
       <c r="J39" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K39" s="18">
         <v>45308.0</v>
       </c>
       <c r="L39" s="17">
         <f t="shared" si="2"/>
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="M39" s="17">
         <v>1740.0</v>
@@ -3419,7 +3422,7 @@
       <c r="AG39" s="1"/>
       <c r="AH39" s="1"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1">
+    <row r="40" ht="15.75" hidden="1" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="13">
         <v>37.0</v>
@@ -3441,14 +3444,14 @@
       <c r="I40" s="13"/>
       <c r="J40" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K40" s="18">
         <v>45308.0</v>
       </c>
       <c r="L40" s="17">
         <f t="shared" si="2"/>
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="M40" s="17">
         <v>1740.0</v>
@@ -3499,14 +3502,14 @@
       <c r="I41" s="13"/>
       <c r="J41" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K41" s="18">
         <v>45378.0</v>
       </c>
       <c r="L41" s="17">
         <f t="shared" si="2"/>
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="M41" s="17">
         <v>1740.0</v>
@@ -3559,14 +3562,14 @@
       <c r="I42" s="13"/>
       <c r="J42" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K42" s="18">
         <v>45291.0</v>
       </c>
       <c r="L42" s="17">
         <f t="shared" si="2"/>
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="M42" s="17">
         <v>1740.0</v>
@@ -3593,7 +3596,7 @@
       <c r="AG42" s="1"/>
       <c r="AH42" s="1"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1">
+    <row r="43" ht="15.75" hidden="1" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="17">
         <v>40.0</v>
@@ -3615,14 +3618,14 @@
       <c r="I43" s="13"/>
       <c r="J43" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K43" s="18">
         <v>45321.0</v>
       </c>
       <c r="L43" s="17">
         <f t="shared" si="2"/>
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="M43" s="17">
         <v>1740.0</v>
@@ -3651,7 +3654,7 @@
       <c r="AG43" s="1"/>
       <c r="AH43" s="1"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
+    <row r="44" ht="15.75" hidden="1" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="13">
         <v>41.0</v>
@@ -3675,14 +3678,14 @@
       <c r="I44" s="13"/>
       <c r="J44" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K44" s="18">
         <v>45475.0</v>
       </c>
       <c r="L44" s="17">
         <f t="shared" si="2"/>
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="M44" s="17">
         <v>1392.0</v>
@@ -3735,14 +3738,14 @@
       <c r="I45" s="13"/>
       <c r="J45" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K45" s="18">
         <v>45475.0</v>
       </c>
       <c r="L45" s="17">
         <f t="shared" si="2"/>
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="M45" s="17">
         <v>1740.0</v>
@@ -3771,7 +3774,7 @@
       <c r="AG45" s="1"/>
       <c r="AH45" s="1"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
+    <row r="46" ht="15.75" hidden="1" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="13">
         <v>43.0</v>
@@ -3793,14 +3796,14 @@
       <c r="I46" s="13"/>
       <c r="J46" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K46" s="18">
         <v>45197.0</v>
       </c>
       <c r="L46" s="17">
         <f t="shared" si="2"/>
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="M46" s="17">
         <v>1392.0</v>
@@ -3827,7 +3830,7 @@
       <c r="AG46" s="1"/>
       <c r="AH46" s="1"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
+    <row r="47" ht="15.75" hidden="1" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="17">
         <v>44.0</v>
@@ -3849,14 +3852,14 @@
       <c r="I47" s="13"/>
       <c r="J47" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K47" s="18">
         <v>45197.0</v>
       </c>
       <c r="L47" s="17">
         <f t="shared" si="2"/>
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="M47" s="17">
         <v>1740.0</v>
@@ -3883,7 +3886,7 @@
       <c r="AG47" s="1"/>
       <c r="AH47" s="1"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" ht="15.75" hidden="1" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="13">
         <v>45.0</v>
@@ -3905,14 +3908,14 @@
       <c r="I48" s="13"/>
       <c r="J48" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K48" s="18">
         <v>45197.0</v>
       </c>
       <c r="L48" s="17">
         <f t="shared" si="2"/>
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="M48" s="17">
         <v>1392.0</v>
@@ -3939,7 +3942,7 @@
       <c r="AG48" s="1"/>
       <c r="AH48" s="1"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
+    <row r="49" ht="15.75" hidden="1" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="17">
         <v>46.0</v>
@@ -3961,14 +3964,14 @@
       <c r="I49" s="13"/>
       <c r="J49" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K49" s="18">
         <v>45197.0</v>
       </c>
       <c r="L49" s="17">
         <f t="shared" si="2"/>
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="M49" s="17">
         <v>1740.0</v>
@@ -4019,14 +4022,14 @@
       <c r="I50" s="13"/>
       <c r="J50" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K50" s="18">
         <v>45340.0</v>
       </c>
       <c r="L50" s="17">
         <f t="shared" si="2"/>
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="M50" s="17">
         <v>1392.0</v>
@@ -4055,7 +4058,7 @@
       <c r="AG50" s="1"/>
       <c r="AH50" s="1"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" ht="15.75" hidden="1" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="17">
         <v>48.0</v>
@@ -4077,14 +4080,14 @@
       <c r="I51" s="13"/>
       <c r="J51" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K51" s="18">
         <v>45336.0</v>
       </c>
       <c r="L51" s="17">
         <f t="shared" si="2"/>
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="M51" s="17">
         <v>1392.0</v>
@@ -4111,7 +4114,7 @@
       <c r="AG51" s="1"/>
       <c r="AH51" s="1"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
+    <row r="52" ht="15.75" hidden="1" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="13">
         <v>49.0</v>
@@ -4133,14 +4136,14 @@
       <c r="I52" s="13"/>
       <c r="J52" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K52" s="18">
         <v>45336.0</v>
       </c>
       <c r="L52" s="17">
         <f t="shared" si="2"/>
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="M52" s="17">
         <v>1740.0</v>
@@ -4167,7 +4170,7 @@
       <c r="AG52" s="1"/>
       <c r="AH52" s="1"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
+    <row r="53" ht="15.75" hidden="1" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="17">
         <v>50.0</v>
@@ -4191,14 +4194,14 @@
       <c r="I53" s="13"/>
       <c r="J53" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K53" s="18">
         <v>45309.0</v>
       </c>
       <c r="L53" s="17">
         <f t="shared" si="2"/>
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="M53" s="17">
         <v>1392.0</v>
@@ -4227,7 +4230,7 @@
       <c r="AG53" s="1"/>
       <c r="AH53" s="1"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" ht="15.75" hidden="1" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="13">
         <v>51.0</v>
@@ -4249,14 +4252,14 @@
       <c r="I54" s="13"/>
       <c r="J54" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K54" s="18">
         <v>45311.0</v>
       </c>
       <c r="L54" s="17">
         <f t="shared" si="2"/>
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="M54" s="17">
         <v>1740.0</v>
@@ -4283,7 +4286,7 @@
       <c r="AG54" s="1"/>
       <c r="AH54" s="1"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
+    <row r="55" ht="15.75" hidden="1" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="17">
         <v>52.0</v>
@@ -4305,14 +4308,14 @@
       <c r="I55" s="13"/>
       <c r="J55" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K55" s="18">
         <v>45177.0</v>
       </c>
       <c r="L55" s="17">
         <f t="shared" si="2"/>
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="M55" s="17">
         <v>1392.0</v>
@@ -4339,7 +4342,7 @@
       <c r="AG55" s="1"/>
       <c r="AH55" s="1"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
+    <row r="56" ht="15.75" hidden="1" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="13">
         <v>53.0</v>
@@ -4361,14 +4364,14 @@
       <c r="I56" s="13"/>
       <c r="J56" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K56" s="18">
         <v>45177.0</v>
       </c>
       <c r="L56" s="17">
         <f t="shared" si="2"/>
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="M56" s="17">
         <v>1740.0</v>
@@ -4421,14 +4424,14 @@
       </c>
       <c r="J57" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K57" s="18">
         <v>45360.0</v>
       </c>
       <c r="L57" s="17">
         <f t="shared" si="2"/>
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="M57" s="17">
         <v>1392.0</v>
@@ -4481,14 +4484,14 @@
       <c r="I58" s="17"/>
       <c r="J58" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K58" s="18">
         <v>45354.0</v>
       </c>
       <c r="L58" s="17">
         <f t="shared" si="2"/>
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="M58" s="17">
         <v>1740.0</v>
@@ -4517,7 +4520,7 @@
       <c r="AG58" s="1"/>
       <c r="AH58" s="1"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
+    <row r="59" ht="15.75" hidden="1" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="17">
         <v>58.0</v>
@@ -4541,14 +4544,14 @@
       <c r="I59" s="17"/>
       <c r="J59" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K59" s="18">
         <v>45354.0</v>
       </c>
       <c r="L59" s="17">
         <f t="shared" si="2"/>
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="M59" s="17">
         <v>1392.0</v>
@@ -4577,7 +4580,7 @@
       <c r="AG59" s="1"/>
       <c r="AH59" s="1"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
+    <row r="60" ht="15.75" hidden="1" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="17">
         <v>60.0</v>
@@ -4599,14 +4602,14 @@
       <c r="I60" s="17"/>
       <c r="J60" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K60" s="18">
         <v>45358.0</v>
       </c>
       <c r="L60" s="17">
         <f t="shared" si="2"/>
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="M60" s="17">
         <v>1740.0</v>
@@ -4657,14 +4660,14 @@
       <c r="I61" s="17"/>
       <c r="J61" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K61" s="18">
         <v>45366.0</v>
       </c>
       <c r="L61" s="17">
         <f t="shared" si="2"/>
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="M61" s="17">
         <v>1740.0</v>
@@ -4693,7 +4696,7 @@
       <c r="AG61" s="1"/>
       <c r="AH61" s="1"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
+    <row r="62" ht="15.75" hidden="1" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="17">
         <v>64.0</v>
@@ -4715,14 +4718,14 @@
       <c r="I62" s="17"/>
       <c r="J62" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K62" s="18">
         <v>45366.0</v>
       </c>
       <c r="L62" s="17">
         <f t="shared" si="2"/>
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="M62" s="17">
         <v>1740.0</v>
@@ -4775,14 +4778,14 @@
       <c r="I63" s="17"/>
       <c r="J63" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K63" s="18">
         <v>45368.0</v>
       </c>
       <c r="L63" s="17">
         <f t="shared" si="2"/>
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M63" s="17">
         <v>3190.0</v>
@@ -4835,14 +4838,14 @@
       <c r="I64" s="17"/>
       <c r="J64" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K64" s="18">
         <v>45368.0</v>
       </c>
       <c r="L64" s="17">
         <f t="shared" si="2"/>
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="M64" s="17">
         <v>1740.0</v>
@@ -4897,14 +4900,14 @@
       </c>
       <c r="J65" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K65" s="18">
         <v>45382.0</v>
       </c>
       <c r="L65" s="17">
         <f t="shared" si="2"/>
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="M65" s="17">
         <v>1740.0</v>
@@ -4933,7 +4936,7 @@
       <c r="AG65" s="1"/>
       <c r="AH65" s="1"/>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
+    <row r="66" ht="15.75" hidden="1" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="17">
         <v>71.0</v>
@@ -4959,14 +4962,14 @@
       </c>
       <c r="J66" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K66" s="18">
         <v>45382.0</v>
       </c>
       <c r="L66" s="17">
         <f t="shared" si="2"/>
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="M66" s="17">
         <v>1392.0</v>
@@ -4995,7 +4998,7 @@
       <c r="AG66" s="1"/>
       <c r="AH66" s="1"/>
     </row>
-    <row r="67" ht="15.75" customHeight="1">
+    <row r="67" ht="15.75" hidden="1" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="17">
         <v>72.0</v>
@@ -5021,14 +5024,14 @@
       </c>
       <c r="J67" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K67" s="18">
         <v>45434.0</v>
       </c>
       <c r="L67" s="17">
         <f t="shared" si="2"/>
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="M67" s="17">
         <v>1392.0</v>
@@ -5057,7 +5060,7 @@
       <c r="AG67" s="1"/>
       <c r="AH67" s="1"/>
     </row>
-    <row r="68" ht="15.75" customHeight="1">
+    <row r="68" ht="15.75" hidden="1" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="17">
         <v>73.0</v>
@@ -5083,14 +5086,14 @@
       </c>
       <c r="J68" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K68" s="18">
         <v>45434.0</v>
       </c>
       <c r="L68" s="17">
         <f t="shared" si="2"/>
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="M68" s="17">
         <v>1740.0</v>
@@ -5119,7 +5122,7 @@
       <c r="AG68" s="1"/>
       <c r="AH68" s="1"/>
     </row>
-    <row r="69" ht="15.75" customHeight="1">
+    <row r="69" ht="15.75" hidden="1" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="17">
         <v>74.0</v>
@@ -5145,14 +5148,14 @@
       </c>
       <c r="J69" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K69" s="18">
         <v>45434.0</v>
       </c>
       <c r="L69" s="17">
         <f t="shared" si="2"/>
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="M69" s="17">
         <v>1740.0</v>
@@ -5186,7 +5189,7 @@
       <c r="B70" s="17">
         <v>76.0</v>
       </c>
-      <c r="C70" s="41" t="s">
+      <c r="C70" s="20" t="s">
         <v>95</v>
       </c>
       <c r="D70" s="21" t="s">
@@ -5207,14 +5210,14 @@
       </c>
       <c r="J70" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K70" s="18">
         <v>45538.0</v>
       </c>
       <c r="L70" s="17">
         <f t="shared" si="2"/>
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="M70" s="17">
         <v>1599.0</v>
@@ -5243,12 +5246,12 @@
       <c r="AG70" s="1"/>
       <c r="AH70" s="1"/>
     </row>
-    <row r="71" ht="15.75" customHeight="1">
+    <row r="71" ht="15.75" hidden="1" customHeight="1">
       <c r="A71" s="1"/>
       <c r="B71" s="17">
         <v>78.0</v>
       </c>
-      <c r="C71" s="42" t="s">
+      <c r="C71" s="20" t="s">
         <v>96</v>
       </c>
       <c r="D71" s="21" t="s">
@@ -5269,14 +5272,14 @@
       </c>
       <c r="J71" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K71" s="18">
         <v>45463.0</v>
       </c>
       <c r="L71" s="17">
         <f t="shared" si="2"/>
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="M71" s="17">
         <v>1392.0</v>
@@ -5310,7 +5313,9 @@
       <c r="B72" s="17">
         <v>80.0</v>
       </c>
-      <c r="C72" s="1"/>
+      <c r="C72" s="32" t="s">
+        <v>97</v>
+      </c>
       <c r="D72" s="21" t="s">
         <v>34</v>
       </c>
@@ -5329,20 +5334,20 @@
       </c>
       <c r="J72" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K72" s="18">
         <v>45540.0</v>
       </c>
       <c r="L72" s="17">
         <f t="shared" si="2"/>
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="M72" s="17">
         <v>1599.0</v>
       </c>
       <c r="N72" s="19" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="O72" s="1"/>
       <c r="P72" s="1"/>
@@ -5365,17 +5370,19 @@
       <c r="AG72" s="1"/>
       <c r="AH72" s="1"/>
     </row>
-    <row r="73" ht="15.75" customHeight="1">
+    <row r="73" ht="15.75" hidden="1" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="17">
         <v>82.0</v>
       </c>
-      <c r="C73" s="1"/>
+      <c r="C73" s="41" t="s">
+        <v>98</v>
+      </c>
       <c r="D73" s="21" t="s">
         <v>34</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F73" s="18">
         <v>45099.0</v>
@@ -5389,20 +5396,20 @@
       </c>
       <c r="J73" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K73" s="18">
         <v>45541.0</v>
       </c>
       <c r="L73" s="17">
         <f t="shared" si="2"/>
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="M73" s="17">
         <v>1599.0</v>
       </c>
       <c r="N73" s="19" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="O73" s="1"/>
       <c r="P73" s="1"/>
@@ -5425,17 +5432,17 @@
       <c r="AG73" s="1"/>
       <c r="AH73" s="1"/>
     </row>
-    <row r="74" ht="15.75" customHeight="1">
+    <row r="74" ht="15.75" hidden="1" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="17">
         <v>84.0</v>
       </c>
-      <c r="C74" s="1"/>
+      <c r="C74" s="42"/>
       <c r="D74" s="21" t="s">
         <v>34</v>
       </c>
       <c r="E74" s="17" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="F74" s="18">
         <v>45100.0</v>
@@ -5449,14 +5456,14 @@
       </c>
       <c r="J74" s="16">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="K74" s="18">
         <v>45542.0</v>
       </c>
       <c r="L74" s="17">
         <f t="shared" si="2"/>
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="M74" s="17">
         <v>1599.0</v>
@@ -37958,6 +37965,14 @@
       <c r="AH976" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="$B$2:$N$74">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Active"/>
+        <filter val="WEBSITE &#10;STATUS"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B2:N2"/>
   </mergeCells>
@@ -38047,15 +38062,1385 @@
     <hyperlink r:id="rId66" ref="C69"/>
     <hyperlink r:id="rId67" ref="C70"/>
     <hyperlink r:id="rId68" ref="C71"/>
+    <hyperlink r:id="rId69" ref="C72"/>
+    <hyperlink r:id="rId70" ref="C73"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId69"/>
+  <drawing r:id="rId71"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="13">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="16">
+        <v>42549.0</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="13"/>
+      <c r="I2" s="16">
+        <f t="shared" ref="I2:I33" si="1">TODAY()</f>
+        <v>45131</v>
+      </c>
+      <c r="J2" s="18">
+        <v>45413.0</v>
+      </c>
+      <c r="K2" s="17">
+        <f t="shared" ref="K2:K33" si="2">J2-I2</f>
+        <v>282</v>
+      </c>
+      <c r="L2" s="17">
+        <v>1549.76</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="13">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="16">
+        <v>42591.0</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J3" s="18">
+        <v>45413.0</v>
+      </c>
+      <c r="K3" s="17">
+        <f t="shared" si="2"/>
+        <v>282</v>
+      </c>
+      <c r="L3" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="16">
+        <v>44246.0</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="I4" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J4" s="16">
+        <v>45706.0</v>
+      </c>
+      <c r="K4" s="17">
+        <f t="shared" si="2"/>
+        <v>575</v>
+      </c>
+      <c r="L4" s="17">
+        <v>3480.0</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="17">
+        <v>6.0</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="16">
+        <v>44874.0</v>
+      </c>
+      <c r="F5" s="17"/>
+      <c r="G5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J5" s="16">
+        <v>45237.0</v>
+      </c>
+      <c r="K5" s="17">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="L5" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="13">
+        <v>7.0</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="16">
+        <v>44785.0</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J6" s="16">
+        <v>45150.0</v>
+      </c>
+      <c r="K6" s="17">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="L6" s="17">
+        <v>1549.76</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="17">
+        <v>8.0</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="18">
+        <v>44260.0</v>
+      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J7" s="18">
+        <v>45721.0</v>
+      </c>
+      <c r="K7" s="17">
+        <f t="shared" si="2"/>
+        <v>590</v>
+      </c>
+      <c r="L7" s="17">
+        <v>2900.0</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="17">
+        <v>10.0</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="18">
+        <v>44463.0</v>
+      </c>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J8" s="18">
+        <v>45189.0</v>
+      </c>
+      <c r="K8" s="17">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="L8" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="13">
+        <v>11.0</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="18">
+        <v>44834.0</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J9" s="18">
+        <v>45198.0</v>
+      </c>
+      <c r="K9" s="17">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="L9" s="17">
+        <v>1392.0</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="17">
+        <v>12.0</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="18">
+        <v>44834.0</v>
+      </c>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J10" s="18">
+        <v>45198.0</v>
+      </c>
+      <c r="K10" s="17">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="L10" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="17">
+        <v>14.0</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="13"/>
+      <c r="I11" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J11" s="18">
+        <v>45198.0</v>
+      </c>
+      <c r="K11" s="17">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="L11" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="13">
+        <v>15.0</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="18">
+        <v>44900.0</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="13"/>
+      <c r="I12" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J12" s="18">
+        <v>45265.0</v>
+      </c>
+      <c r="K12" s="17">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="L12" s="17">
+        <v>1392.0</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="17">
+        <v>16.0</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="18">
+        <v>43894.0</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="13"/>
+      <c r="I13" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J13" s="18">
+        <v>45355.0</v>
+      </c>
+      <c r="K13" s="17">
+        <f t="shared" si="2"/>
+        <v>224</v>
+      </c>
+      <c r="L13" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="17">
+        <v>18.0</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="18">
+        <v>44945.0</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J14" s="18">
+        <v>45309.0</v>
+      </c>
+      <c r="K14" s="17">
+        <f t="shared" si="2"/>
+        <v>178</v>
+      </c>
+      <c r="L14" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M14" s="19"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="13">
+        <v>21.0</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="18">
+        <v>44900.0</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J15" s="18">
+        <v>45265.0</v>
+      </c>
+      <c r="K15" s="17">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="L15" s="17">
+        <v>1392.0</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="17">
+        <v>22.0</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="18">
+        <v>44616.0</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J16" s="18">
+        <v>45345.0</v>
+      </c>
+      <c r="K16" s="17">
+        <f t="shared" si="2"/>
+        <v>214</v>
+      </c>
+      <c r="L16" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M16" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="17">
+        <v>24.0</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="18">
+        <v>42314.0</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J17" s="18">
+        <v>45494.0</v>
+      </c>
+      <c r="K17" s="17">
+        <f t="shared" si="2"/>
+        <v>363</v>
+      </c>
+      <c r="L17" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M17" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="13">
+        <v>25.0</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="18">
+        <v>41811.0</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J18" s="18">
+        <v>45343.0</v>
+      </c>
+      <c r="K18" s="17">
+        <f t="shared" si="2"/>
+        <v>212</v>
+      </c>
+      <c r="L18" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M18" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="13">
+        <v>33.0</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="18">
+        <v>44387.0</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J19" s="18">
+        <v>45479.0</v>
+      </c>
+      <c r="K19" s="17">
+        <f t="shared" si="2"/>
+        <v>348</v>
+      </c>
+      <c r="L19" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M19" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="17">
+        <v>34.0</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="18">
+        <v>44963.0</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J20" s="18">
+        <v>45328.0</v>
+      </c>
+      <c r="K20" s="17">
+        <f t="shared" si="2"/>
+        <v>197</v>
+      </c>
+      <c r="L20" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M20" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="17">
+        <v>36.0</v>
+      </c>
+      <c r="B21" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="18">
+        <v>43482.0</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="13"/>
+      <c r="I21" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J21" s="18">
+        <v>45308.0</v>
+      </c>
+      <c r="K21" s="17">
+        <f t="shared" si="2"/>
+        <v>177</v>
+      </c>
+      <c r="L21" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M21" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="17">
+        <v>38.0</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="18">
+        <v>43917.0</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J22" s="18">
+        <v>45378.0</v>
+      </c>
+      <c r="K22" s="17">
+        <f t="shared" si="2"/>
+        <v>247</v>
+      </c>
+      <c r="L22" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M22" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="13">
+        <v>39.0</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="18">
+        <v>44935.0</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="13"/>
+      <c r="I23" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J23" s="18">
+        <v>45291.0</v>
+      </c>
+      <c r="K23" s="17">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="L23" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M23" s="19"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="17">
+        <v>42.0</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="18">
+        <v>44014.0</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="I24" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J24" s="18">
+        <v>45475.0</v>
+      </c>
+      <c r="K24" s="17">
+        <f t="shared" si="2"/>
+        <v>344</v>
+      </c>
+      <c r="L24" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M24" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="13">
+        <v>47.0</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="18">
+        <v>44610.0</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="13"/>
+      <c r="I25" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J25" s="18">
+        <v>45340.0</v>
+      </c>
+      <c r="K25" s="17">
+        <f t="shared" si="2"/>
+        <v>209</v>
+      </c>
+      <c r="L25" s="17">
+        <v>1392.0</v>
+      </c>
+      <c r="M25" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="17">
+        <v>54.0</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="18">
+        <v>44994.0</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J26" s="18">
+        <v>45360.0</v>
+      </c>
+      <c r="K26" s="17">
+        <f t="shared" si="2"/>
+        <v>229</v>
+      </c>
+      <c r="L26" s="17">
+        <v>1392.0</v>
+      </c>
+      <c r="M26" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="17">
+        <v>56.0</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="18">
+        <v>44988.0</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="17"/>
+      <c r="I27" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J27" s="18">
+        <v>45354.0</v>
+      </c>
+      <c r="K27" s="17">
+        <f t="shared" si="2"/>
+        <v>223</v>
+      </c>
+      <c r="L27" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M27" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="17">
+        <v>62.0</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="18">
+        <v>45000.0</v>
+      </c>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J28" s="18">
+        <v>45366.0</v>
+      </c>
+      <c r="K28" s="17">
+        <f t="shared" si="2"/>
+        <v>235</v>
+      </c>
+      <c r="L28" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M28" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="17">
+        <v>66.0</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="18">
+        <v>45002.0</v>
+      </c>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" s="17"/>
+      <c r="I29" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J29" s="18">
+        <v>45368.0</v>
+      </c>
+      <c r="K29" s="17">
+        <f t="shared" si="2"/>
+        <v>237</v>
+      </c>
+      <c r="L29" s="17">
+        <v>3190.0</v>
+      </c>
+      <c r="M29" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="17">
+        <v>68.0</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="18">
+        <v>45002.0</v>
+      </c>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30" s="17"/>
+      <c r="I30" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J30" s="18">
+        <v>45368.0</v>
+      </c>
+      <c r="K30" s="17">
+        <f t="shared" si="2"/>
+        <v>237</v>
+      </c>
+      <c r="L30" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M30" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="17">
+        <v>70.0</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="18">
+        <v>45016.0</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J31" s="18">
+        <v>45382.0</v>
+      </c>
+      <c r="K31" s="17">
+        <f t="shared" si="2"/>
+        <v>251</v>
+      </c>
+      <c r="L31" s="17">
+        <v>1740.0</v>
+      </c>
+      <c r="M31" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="17">
+        <v>76.0</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="18">
+        <v>40799.0</v>
+      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J32" s="18">
+        <v>45538.0</v>
+      </c>
+      <c r="K32" s="17">
+        <f t="shared" si="2"/>
+        <v>407</v>
+      </c>
+      <c r="L32" s="17">
+        <v>1599.0</v>
+      </c>
+      <c r="M32" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="17">
+        <v>80.0</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="18">
+        <v>45098.0</v>
+      </c>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33" s="16">
+        <f t="shared" si="1"/>
+        <v>45131</v>
+      </c>
+      <c r="J33" s="18">
+        <v>45540.0</v>
+      </c>
+      <c r="K33" s="17">
+        <f t="shared" si="2"/>
+        <v>409</v>
+      </c>
+      <c r="L33" s="17">
+        <v>1599.0</v>
+      </c>
+      <c r="M33" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2:H33">
+      <formula1>"Klif,Michael,Fabian,Warren,Hardy"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D33">
+      <formula1>"Active,Inactive"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C33">
+      <formula1>"Deep Africa,Sasahost,Host Africa"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F2:F33">
+      <formula1>"Contabo,Hostgator,Deep Africa,Sasahost,No Host"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M2:M33">
+      <formula1>"CM Advocates,Bellmac,Riskhouse,Property Boutique"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink r:id="rId3" ref="B4"/>
+    <hyperlink r:id="rId4" ref="B5"/>
+    <hyperlink r:id="rId5" ref="B6"/>
+    <hyperlink r:id="rId6" ref="B7"/>
+    <hyperlink r:id="rId7" ref="B8"/>
+    <hyperlink r:id="rId8" ref="B9"/>
+    <hyperlink r:id="rId9" ref="B10"/>
+    <hyperlink r:id="rId10" ref="B11"/>
+    <hyperlink r:id="rId11" ref="B12"/>
+    <hyperlink r:id="rId12" ref="B13"/>
+    <hyperlink r:id="rId13" ref="B14"/>
+    <hyperlink r:id="rId14" ref="B15"/>
+    <hyperlink r:id="rId15" ref="B16"/>
+    <hyperlink r:id="rId16" ref="B17"/>
+    <hyperlink r:id="rId17" ref="B18"/>
+    <hyperlink r:id="rId18" ref="B19"/>
+    <hyperlink r:id="rId19" ref="B20"/>
+    <hyperlink r:id="rId20" ref="B21"/>
+    <hyperlink r:id="rId21" ref="B22"/>
+    <hyperlink r:id="rId22" ref="B23"/>
+    <hyperlink r:id="rId23" ref="B24"/>
+    <hyperlink r:id="rId24" ref="B25"/>
+    <hyperlink r:id="rId25" ref="B26"/>
+    <hyperlink r:id="rId26" ref="B27"/>
+    <hyperlink r:id="rId27" ref="B28"/>
+    <hyperlink r:id="rId28" ref="B29"/>
+    <hyperlink r:id="rId29" ref="B30"/>
+    <hyperlink r:id="rId30" ref="B31"/>
+    <hyperlink r:id="rId31" ref="B32"/>
+    <hyperlink r:id="rId32" ref="B33"/>
+  </hyperlinks>
+  <drawing r:id="rId33"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -38108,7 +39493,7 @@
     <row r="2">
       <c r="A2" s="43"/>
       <c r="B2" s="47" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -38140,31 +39525,31 @@
     <row r="3" ht="33.75" customHeight="1">
       <c r="A3" s="43"/>
       <c r="B3" s="48" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D3" s="50" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G3" s="49" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H3" s="49" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="49" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K3" s="43"/>
       <c r="L3" s="43"/>
@@ -38191,33 +39576,33 @@
         <v>20</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D4" s="54">
         <v>44658.0</v>
       </c>
       <c r="E4" s="54">
         <f t="shared" ref="E4:E14" si="1">TODAY()</f>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="F4" s="54">
         <v>45053.0</v>
       </c>
       <c r="G4" s="55">
         <f t="shared" ref="G4:G10" si="2">F4-E4</f>
-        <v>-71</v>
+        <v>-78</v>
       </c>
       <c r="H4" s="56" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I4" s="53" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J4" s="57">
         <v>103.0</v>
       </c>
       <c r="K4" s="58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L4" s="43"/>
       <c r="M4" s="43"/>
@@ -38241,21 +39626,21 @@
       <c r="A5" s="43"/>
       <c r="B5" s="59"/>
       <c r="C5" s="53" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D5" s="54">
         <v>44984.0</v>
       </c>
       <c r="E5" s="54">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="F5" s="54">
         <v>45349.0</v>
       </c>
       <c r="G5" s="55">
         <f t="shared" si="2"/>
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="H5" s="56" t="s">
         <v>17</v>
@@ -38286,36 +39671,36 @@
     <row r="6">
       <c r="A6" s="43"/>
       <c r="B6" s="52" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D6" s="54">
         <v>44634.0</v>
       </c>
       <c r="E6" s="54">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="F6" s="54">
         <v>45030.0</v>
       </c>
       <c r="G6" s="55">
         <f t="shared" si="2"/>
-        <v>-94</v>
+        <v>-101</v>
       </c>
       <c r="H6" s="56" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I6" s="60" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J6" s="57">
         <v>53.0</v>
       </c>
       <c r="K6" s="58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L6" s="43"/>
       <c r="M6" s="43"/>
@@ -38339,27 +39724,27 @@
       <c r="A7" s="43"/>
       <c r="B7" s="59"/>
       <c r="C7" s="53" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D7" s="54">
         <v>44636.0</v>
       </c>
       <c r="E7" s="54">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="F7" s="54">
         <v>45032.0</v>
       </c>
       <c r="G7" s="55">
         <f t="shared" si="2"/>
-        <v>-92</v>
+        <v>-99</v>
       </c>
       <c r="H7" s="56" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I7" s="60" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J7" s="61"/>
       <c r="K7" s="43"/>
@@ -38384,24 +39769,24 @@
     <row r="8">
       <c r="A8" s="43"/>
       <c r="B8" s="52" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D8" s="54">
         <v>44689.0</v>
       </c>
       <c r="E8" s="54">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="F8" s="54">
         <v>45085.0</v>
       </c>
       <c r="G8" s="55">
         <f t="shared" si="2"/>
-        <v>-39</v>
+        <v>-46</v>
       </c>
       <c r="H8" s="62" t="s">
         <v>17</v>
@@ -38413,7 +39798,7 @@
         <v>23.0</v>
       </c>
       <c r="K8" s="58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L8" s="43"/>
       <c r="M8" s="43"/>
@@ -38437,24 +39822,24 @@
       <c r="A9" s="43"/>
       <c r="B9" s="59"/>
       <c r="C9" s="53" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D9" s="54">
         <v>44662.0</v>
       </c>
       <c r="E9" s="54">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="F9" s="54">
         <v>45057.0</v>
       </c>
       <c r="G9" s="55">
         <f t="shared" si="2"/>
-        <v>-67</v>
+        <v>-74</v>
       </c>
       <c r="H9" s="56" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I9" s="64"/>
       <c r="J9" s="57">
@@ -38482,24 +39867,24 @@
     <row r="10">
       <c r="A10" s="43"/>
       <c r="B10" s="65" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D10" s="54">
         <v>44692.0</v>
       </c>
       <c r="E10" s="54">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="F10" s="54">
         <v>45088.0</v>
       </c>
       <c r="G10" s="55">
         <f t="shared" si="2"/>
-        <v>-36</v>
+        <v>-43</v>
       </c>
       <c r="H10" s="62" t="s">
         <v>17</v>
@@ -38511,7 +39896,7 @@
         <v>23.0</v>
       </c>
       <c r="K10" s="58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L10" s="43"/>
       <c r="M10" s="43"/>
@@ -38537,26 +39922,26 @@
         <v>22</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D11" s="66"/>
       <c r="E11" s="54">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="F11" s="66"/>
       <c r="G11" s="55">
         <v>0.0</v>
       </c>
       <c r="H11" s="67" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I11" s="60" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J11" s="61"/>
       <c r="K11" s="58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L11" s="43"/>
       <c r="M11" s="43"/>
@@ -38580,21 +39965,21 @@
       <c r="A12" s="43"/>
       <c r="B12" s="59"/>
       <c r="C12" s="53" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D12" s="54">
         <v>44860.0</v>
       </c>
       <c r="E12" s="54">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="F12" s="54">
         <v>45225.0</v>
       </c>
       <c r="G12" s="55">
         <f>F12-E12</f>
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="H12" s="67" t="s">
         <v>17</v>
@@ -38628,26 +40013,26 @@
         <v>90</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D13" s="66"/>
       <c r="E13" s="54">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="F13" s="66"/>
       <c r="G13" s="55">
         <v>0.0</v>
       </c>
       <c r="H13" s="67" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I13" s="60" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J13" s="61"/>
       <c r="K13" s="58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="L13" s="43"/>
       <c r="M13" s="43"/>
@@ -38670,24 +40055,24 @@
     <row r="14">
       <c r="A14" s="43"/>
       <c r="B14" s="52" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C14" s="53" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D14" s="54">
         <v>44681.0</v>
       </c>
       <c r="E14" s="54">
         <f t="shared" si="1"/>
-        <v>45124</v>
+        <v>45131</v>
       </c>
       <c r="F14" s="54">
         <v>45076.0</v>
       </c>
       <c r="G14" s="55">
         <f>F14-E14</f>
-        <v>-48</v>
+        <v>-55</v>
       </c>
       <c r="H14" s="62" t="s">
         <v>17</v>
@@ -38721,7 +40106,7 @@
       <c r="A15" s="43"/>
       <c r="B15" s="68"/>
       <c r="C15" s="69" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D15" s="70"/>
       <c r="E15" s="70"/>
@@ -38755,7 +40140,7 @@
       <c r="A16" s="43"/>
       <c r="B16" s="68"/>
       <c r="C16" s="69" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D16" s="70"/>
       <c r="E16" s="70"/>
@@ -38789,7 +40174,7 @@
       <c r="A17" s="43"/>
       <c r="B17" s="68"/>
       <c r="C17" s="69" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D17" s="70"/>
       <c r="E17" s="70"/>
@@ -38821,7 +40206,7 @@
       <c r="A18" s="43"/>
       <c r="B18" s="59"/>
       <c r="C18" s="69" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D18" s="70"/>
       <c r="E18" s="70"/>
@@ -38886,7 +40271,7 @@
     <row r="20">
       <c r="A20" s="43"/>
       <c r="B20" s="19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C20" s="71"/>
       <c r="D20" s="70"/>
@@ -38894,7 +40279,7 @@
       <c r="F20" s="70"/>
       <c r="G20" s="70"/>
       <c r="H20" s="69" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I20" s="71"/>
       <c r="J20" s="72"/>

</xml_diff>